<commit_message>
add default_preference_duration in xlsx
</commit_message>
<xml_diff>
--- a/FlOpEDT/media/configuration/empty_database_file.xlsx
+++ b/FlOpEDT/media/configuration/empty_database_file.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="95">
   <si>
     <t xml:space="preserve">Liste intervenants</t>
   </si>
@@ -301,16 +301,26 @@
   </si>
   <si>
     <t xml:space="preserve">Fin de la pause déjeuner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Granularité des disponibilités</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Définit la taille des blocs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(en min)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="HH:MM"/>
+    <numFmt numFmtId="167" formatCode="#,##0"/>
   </numFmts>
   <fonts count="11">
     <font>
@@ -545,7 +555,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -715,6 +725,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="9" fillId="10" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="9" fillId="10" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -992,10 +1006,10 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="12.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="8.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2004,7 +2018,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="31.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="22.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="20.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="8.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2104,7 +2118,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.29"/>
@@ -2114,12 +2128,12 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="20.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="17.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="14.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="11" style="0" width="8.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="11" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="28.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="24.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="8.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="25.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="17" style="0" width="8.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="17" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2518,9 +2532,9 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="3" style="0" width="8.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="3" style="0" width="8.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="8.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="8.21"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3128,16 +3142,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="false" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="34.59"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="38" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="3" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="18.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="13" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3225,6 +3242,23 @@
       </c>
       <c r="B5" s="42" t="n">
         <v>0.583333333333333</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="40" t="s">
+        <v>92</v>
+      </c>
+      <c r="B7" s="43" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Second version of a checker code for the description of a database file
</commit_message>
<xml_diff>
--- a/FlOpEDT/media/configuration/empty_database_file.xlsx
+++ b/FlOpEDT/media/configuration/empty_database_file.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Paramètres" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="70">
   <si>
     <t xml:space="preserve">Dans cette feuille, trois sous-tableaux apparaissent.</t>
   </si>
@@ -36,7 +36,7 @@
     <t xml:space="preserve">Le dernier est par nature extensible : il ne faut pas toucher à l’entête mais les lignes peuvent être ajoutées, enlevées, laissées vides.</t>
   </si>
   <si>
-    <t xml:space="preserve">Dans ce dernier tableau, les identifiants doivent exister et être uniques, sinon la ligne est ignorée</t>
+    <t xml:space="preserve">Dans ce dernier tableau, les identifiants doivent exister, sinon la ligne est ignorée</t>
   </si>
   <si>
     <t xml:space="preserve">Jalon</t>
@@ -102,88 +102,91 @@
     <t xml:space="preserve">Ne pas toucher aux colonnes ou à l’entête</t>
   </si>
   <si>
+    <t xml:space="preserve">Les lignes sans identifiant sont ignorées.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Les identifiants doivent être uniques</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prénom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adresse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Statut</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Employeur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Un groupe de salles est une liste de salles qui seront réservées d’un bloc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Une catégorie de salle est une liste de salles ou de groupes dont l’un sera choisi pour recevoir le cours.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Une liste est donnée en mettant un élément par colonne horizontalement jusqu’à la première case vide.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Les cases Groupes et Catégories servent de délimiteurs pour le traitement automatique : l’une en dessous de l’autre, sur la même colonne, dans le même ordre.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Groupes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Salles concernées</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Catégories</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Salles et groupes concernés</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Les identifiants doivent exister et être uniques (sinon la ligne est ignorée), un identifiant vide signale la fin du tableau</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Promotions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Natures de groupes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Le sur-groupe est celui immédiatement au dessus dans la hiérarchie, s’il y en a.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Les identifiants doivent exister et être uniques (sinon la ligne est ignorée)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Promotion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nature</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sur-groupe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Un module est une charge d’enseignement sur une période et une promotion.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L’abréviation est le nom dans l’emploi du temps.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Le code PPN (Programme Pédagogique National) concerne certaines formations.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Le responsable l’est du point de vue administratif et n’est pas forcément en charge de (tout) l’enseignement.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ne pas toucher aux colonnes ou à l’entête.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Les lignes vides ne sont pas un problème.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Les identifiants doivent exister et être uniques, sinon la ligne est ignorée.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nom</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Prénom</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adresse</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Statut</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Employeur</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Un groupe de salles est une liste de salles qui seront réservées d’un bloc.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Une catégorie de salle est une liste de salles ou de groupes dont l’un sera choisi pour recevoir le cours.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Une liste est donnée en mettant un élément par colonne horizontalement jusqu’à la première case vide.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Les cases Groupes et Catégories servent de délimiteurs pour le traitement automatique : l’une en dessous de l’autre, sur la même colonne, dans le même ordre.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Groupes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Salles concernées</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Catégories</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Salles et groupes concernés</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Les identifiants doivent exister et être uniques (sinon la ligne est ignorée), un identifiant vide signale la fin du tableau</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Promotions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Natures de groupes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Le sur-groupe est celui immédiatement au dessus dans la hiérarchie, s’il y en a.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Les identifiants doivent exister et être uniques (sinon la ligne est ignorée)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Promotion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nature</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sur-groupe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Un module est une charge d’enseignement sur une période et une promotion.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L’abréviation est le nom dans l’emploi du temps.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Le code PPN (Programme Pédagogique National) concerne certaines formations.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Le responsable l’est du point de vue administratif et n’est pas forcément en charge de (tout) l’enseignement.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ne pas toucher aux colonnes ou à l’entête.</t>
   </si>
   <si>
     <t xml:space="preserve">Abréviation</t>
@@ -211,7 +214,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">-  la première donne le nom du type, la durée, puis la liste des types de groupe concernés </t>
+      <t xml:space="preserve">-  la première donne le nom du type, la durée, puis la liste des natures de groupe concernés </t>
     </r>
     <r>
       <rPr>
@@ -277,7 +280,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="HH:MM"/>
+    <numFmt numFmtId="165" formatCode="hh:mm"/>
     <numFmt numFmtId="166" formatCode="@"/>
   </numFmts>
   <fonts count="11">
@@ -590,13 +593,13 @@
     </xf>
   </cellXfs>
   <cellStyles count="7">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Warning 1" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="20"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -672,7 +675,7 @@
       <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.6"/>
   </cols>
@@ -887,10 +890,10 @@
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="8" width="17.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="8" width="9.63"/>
@@ -898,7 +901,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="8" width="30.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="8" width="11.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="8" width="17.83"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="7" style="8" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="7" style="8" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" s="10" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1135,12 +1138,12 @@
       <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="13" width="21.58"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="2" style="13" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="13" width="12.83"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="6" style="13" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="6" style="13" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1465,18 +1468,17 @@
   </sheetPr>
   <dimension ref="A1:AMJ45"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A25" activeCellId="0" sqref="A25"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="8" width="16.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="8" width="29.5"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="8" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="8" width="18.89"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1020" min="5" style="8" width="11.52"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1021" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" s="25" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1769,7 +1771,7 @@
       <selection pane="topLeft" activeCell="F22" activeCellId="0" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="8" width="18.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="8" width="17.21"/>
@@ -1777,7 +1779,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="8" width="17.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="8" width="15.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="8" width="20.6"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="7" style="8" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="7" style="8" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1807,27 +1809,27 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="23" t="s">
-        <v>25</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" s="29" customFormat="true" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>45</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2089,50 +2091,50 @@
   </sheetPr>
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C24" activeCellId="0" sqref="C24"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="30" width="9.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="8" width="19.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="30" width="10.05"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="4" style="30" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="4" style="30" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="30" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="30" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="30" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="30" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="31" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B5" s="32" t="n">
         <v>60</v>
       </c>
       <c r="C5" s="31" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D5" s="31" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E5" s="31"/>
       <c r="F5" s="31"/>
@@ -2155,23 +2157,23 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="34" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="34" t="s">
-        <v>25</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" s="37" customFormat="true" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="35" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C10" s="36" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D10" s="36"/>
       <c r="E10" s="36"/>

</xml_diff>

<commit_message>
first try to consider transversal groups in deploy_database
</commit_message>
<xml_diff>
--- a/FlOpEDT/media/configuration/empty_database_file.xlsx
+++ b/FlOpEDT/media/configuration/empty_database_file.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Paramètres" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="79">
   <si>
     <t xml:space="preserve">Dans cette feuille, trois sous-tableaux apparaissent.</t>
   </si>
@@ -156,12 +156,24 @@
     <t xml:space="preserve">Natures de groupes</t>
   </si>
   <si>
-    <t xml:space="preserve">Le sur-groupe est celui immédiatement au dessus dans la hiérarchie, s’il y en a.</t>
+    <t xml:space="preserve">Le sur-groupe est celui immédiatement au dessus dans la hiérarchie.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Les groupes structuraux d’une promotion doivent former un arbre, donc :</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- chaque groupe a un unique parent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- sauf un unique groupe par promotion,la racine, qui est sans parent et l'ancêtre de tous les autres</t>
   </si>
   <si>
     <t xml:space="preserve">Les identifiants doivent exister et être uniques (sinon la ligne est ignorée)</t>
   </si>
   <si>
+    <t xml:space="preserve">Groupes Structuraux</t>
+  </si>
+  <si>
     <t xml:space="preserve">Promotion</t>
   </si>
   <si>
@@ -169,6 +181,18 @@
   </si>
   <si>
     <t xml:space="preserve">Sur-groupe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Un groupe transversal (ex : groupe d’anglais) est transversal à plusieurs groupes structuraux, et peut être parallèle à plusieurs groupes transversaux (ex : espagnol, allemand…)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Groupes Transversaux</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transversal à quels groupes structuraux ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parallèle à quels groupes transversaux ?</t>
   </si>
   <si>
     <t xml:space="preserve">Un module est une charge d’enseignement sur une période et une promotion.</t>
@@ -433,7 +457,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="42">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -548,6 +572,14 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -901,7 +933,7 @@
   </sheetPr>
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
     </sheetView>
   </sheetViews>
@@ -1478,10 +1510,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ45"/>
+  <dimension ref="A1:AMJ72"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A24" activeCellId="0" sqref="A24"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A11" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A50" activeCellId="0" sqref="A50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1489,7 +1521,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="8" width="16.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="8" width="29.5"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="8" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="8" width="18.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="8" width="11.66"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1020" min="5" style="8" width="11.52"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1021" style="0" width="11.54"/>
   </cols>
@@ -1603,49 +1635,46 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="23" t="s">
+      <c r="A24" s="8" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-    </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="5" t="s">
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="23" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+    </row>
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B27" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="11"/>
-      <c r="B28" s="11"/>
-      <c r="C28" s="11"/>
-      <c r="D28" s="28"/>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="11"/>
-      <c r="B29" s="11"/>
-      <c r="C29" s="11"/>
-      <c r="D29" s="28"/>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="11"/>
-      <c r="B30" s="11"/>
-      <c r="C30" s="11"/>
-      <c r="D30" s="28"/>
+      <c r="B30" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="11"/>
@@ -1737,8 +1766,406 @@
       <c r="C45" s="11"/>
       <c r="D45" s="28"/>
     </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="11"/>
+      <c r="B46" s="11"/>
+      <c r="C46" s="11"/>
+      <c r="D46" s="28"/>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="11"/>
+      <c r="B47" s="11"/>
+      <c r="C47" s="11"/>
+      <c r="D47" s="28"/>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="11"/>
+      <c r="B48" s="11"/>
+      <c r="C48" s="11"/>
+      <c r="D48" s="28"/>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="23" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="29" t="s">
+        <v>53</v>
+      </c>
+      <c r="B53" s="29"/>
+      <c r="C53" s="29"/>
+      <c r="D53" s="29"/>
+      <c r="E53" s="29"/>
+      <c r="F53" s="29"/>
+      <c r="G53" s="29"/>
+      <c r="H53" s="29"/>
+      <c r="I53" s="29"/>
+      <c r="J53" s="29"/>
+      <c r="K53" s="29"/>
+      <c r="L53" s="29"/>
+      <c r="M53" s="29"/>
+      <c r="N53" s="29"/>
+      <c r="O53" s="29"/>
+      <c r="P53" s="29"/>
+    </row>
+    <row r="54" s="8" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C54" s="30" t="s">
+        <v>54</v>
+      </c>
+      <c r="D54" s="30"/>
+      <c r="E54" s="30"/>
+      <c r="F54" s="30"/>
+      <c r="G54" s="30"/>
+      <c r="H54" s="30"/>
+      <c r="I54" s="30"/>
+      <c r="J54" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="K54" s="30"/>
+      <c r="L54" s="30"/>
+      <c r="M54" s="30"/>
+      <c r="N54" s="30"/>
+      <c r="O54" s="30"/>
+      <c r="P54" s="30"/>
+    </row>
+    <row r="55" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="11"/>
+      <c r="B55" s="11"/>
+      <c r="C55" s="11"/>
+      <c r="D55" s="11"/>
+      <c r="E55" s="11"/>
+      <c r="F55" s="11"/>
+      <c r="G55" s="11"/>
+      <c r="H55" s="11"/>
+      <c r="I55" s="11"/>
+      <c r="J55" s="11"/>
+      <c r="K55" s="11"/>
+      <c r="L55" s="11"/>
+      <c r="M55" s="11"/>
+      <c r="N55" s="11"/>
+      <c r="O55" s="11"/>
+      <c r="P55" s="28"/>
+    </row>
+    <row r="56" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="11"/>
+      <c r="B56" s="11"/>
+      <c r="C56" s="11"/>
+      <c r="D56" s="11"/>
+      <c r="E56" s="11"/>
+      <c r="F56" s="11"/>
+      <c r="G56" s="11"/>
+      <c r="H56" s="11"/>
+      <c r="I56" s="11"/>
+      <c r="J56" s="11"/>
+      <c r="K56" s="11"/>
+      <c r="L56" s="11"/>
+      <c r="M56" s="11"/>
+      <c r="N56" s="11"/>
+      <c r="O56" s="11"/>
+      <c r="P56" s="28"/>
+    </row>
+    <row r="57" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="11"/>
+      <c r="B57" s="11"/>
+      <c r="C57" s="11"/>
+      <c r="D57" s="11"/>
+      <c r="E57" s="11"/>
+      <c r="F57" s="11"/>
+      <c r="G57" s="11"/>
+      <c r="H57" s="11"/>
+      <c r="I57" s="11"/>
+      <c r="J57" s="11"/>
+      <c r="K57" s="11"/>
+      <c r="L57" s="11"/>
+      <c r="M57" s="11"/>
+      <c r="N57" s="11"/>
+      <c r="O57" s="11"/>
+      <c r="P57" s="28"/>
+    </row>
+    <row r="58" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="11"/>
+      <c r="B58" s="11"/>
+      <c r="C58" s="11"/>
+      <c r="D58" s="11"/>
+      <c r="E58" s="11"/>
+      <c r="F58" s="11"/>
+      <c r="G58" s="11"/>
+      <c r="H58" s="11"/>
+      <c r="I58" s="11"/>
+      <c r="J58" s="11"/>
+      <c r="K58" s="11"/>
+      <c r="L58" s="11"/>
+      <c r="M58" s="11"/>
+      <c r="N58" s="11"/>
+      <c r="O58" s="11"/>
+      <c r="P58" s="28"/>
+    </row>
+    <row r="59" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="11"/>
+      <c r="B59" s="11"/>
+      <c r="C59" s="11"/>
+      <c r="D59" s="11"/>
+      <c r="E59" s="11"/>
+      <c r="F59" s="11"/>
+      <c r="G59" s="11"/>
+      <c r="H59" s="11"/>
+      <c r="I59" s="11"/>
+      <c r="J59" s="11"/>
+      <c r="K59" s="11"/>
+      <c r="L59" s="11"/>
+      <c r="M59" s="11"/>
+      <c r="N59" s="11"/>
+      <c r="O59" s="11"/>
+      <c r="P59" s="28"/>
+    </row>
+    <row r="60" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="11"/>
+      <c r="B60" s="11"/>
+      <c r="C60" s="11"/>
+      <c r="D60" s="11"/>
+      <c r="E60" s="11"/>
+      <c r="F60" s="11"/>
+      <c r="G60" s="11"/>
+      <c r="H60" s="11"/>
+      <c r="I60" s="11"/>
+      <c r="J60" s="11"/>
+      <c r="K60" s="11"/>
+      <c r="L60" s="11"/>
+      <c r="M60" s="11"/>
+      <c r="N60" s="11"/>
+      <c r="O60" s="11"/>
+      <c r="P60" s="28"/>
+    </row>
+    <row r="61" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="11"/>
+      <c r="B61" s="11"/>
+      <c r="C61" s="11"/>
+      <c r="D61" s="11"/>
+      <c r="E61" s="11"/>
+      <c r="F61" s="11"/>
+      <c r="G61" s="11"/>
+      <c r="H61" s="11"/>
+      <c r="I61" s="11"/>
+      <c r="J61" s="11"/>
+      <c r="K61" s="11"/>
+      <c r="L61" s="11"/>
+      <c r="M61" s="11"/>
+      <c r="N61" s="11"/>
+      <c r="O61" s="11"/>
+      <c r="P61" s="28"/>
+    </row>
+    <row r="62" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="11"/>
+      <c r="B62" s="11"/>
+      <c r="C62" s="11"/>
+      <c r="D62" s="11"/>
+      <c r="E62" s="11"/>
+      <c r="F62" s="11"/>
+      <c r="G62" s="11"/>
+      <c r="H62" s="11"/>
+      <c r="I62" s="11"/>
+      <c r="J62" s="11"/>
+      <c r="K62" s="11"/>
+      <c r="L62" s="11"/>
+      <c r="M62" s="11"/>
+      <c r="N62" s="11"/>
+      <c r="O62" s="11"/>
+      <c r="P62" s="28"/>
+    </row>
+    <row r="63" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="11"/>
+      <c r="B63" s="11"/>
+      <c r="C63" s="11"/>
+      <c r="D63" s="11"/>
+      <c r="E63" s="11"/>
+      <c r="F63" s="11"/>
+      <c r="G63" s="11"/>
+      <c r="H63" s="11"/>
+      <c r="I63" s="11"/>
+      <c r="J63" s="11"/>
+      <c r="K63" s="11"/>
+      <c r="L63" s="11"/>
+      <c r="M63" s="11"/>
+      <c r="N63" s="11"/>
+      <c r="O63" s="11"/>
+      <c r="P63" s="28"/>
+    </row>
+    <row r="64" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="11"/>
+      <c r="B64" s="11"/>
+      <c r="C64" s="11"/>
+      <c r="D64" s="11"/>
+      <c r="E64" s="11"/>
+      <c r="F64" s="11"/>
+      <c r="G64" s="11"/>
+      <c r="H64" s="11"/>
+      <c r="I64" s="11"/>
+      <c r="J64" s="11"/>
+      <c r="K64" s="11"/>
+      <c r="L64" s="11"/>
+      <c r="M64" s="11"/>
+      <c r="N64" s="11"/>
+      <c r="O64" s="11"/>
+      <c r="P64" s="28"/>
+    </row>
+    <row r="65" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="11"/>
+      <c r="B65" s="11"/>
+      <c r="C65" s="11"/>
+      <c r="D65" s="11"/>
+      <c r="E65" s="11"/>
+      <c r="F65" s="11"/>
+      <c r="G65" s="11"/>
+      <c r="H65" s="11"/>
+      <c r="I65" s="11"/>
+      <c r="J65" s="11"/>
+      <c r="K65" s="11"/>
+      <c r="L65" s="11"/>
+      <c r="M65" s="11"/>
+      <c r="N65" s="11"/>
+      <c r="O65" s="11"/>
+      <c r="P65" s="28"/>
+    </row>
+    <row r="66" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="11"/>
+      <c r="B66" s="11"/>
+      <c r="C66" s="11"/>
+      <c r="D66" s="11"/>
+      <c r="E66" s="11"/>
+      <c r="F66" s="11"/>
+      <c r="G66" s="11"/>
+      <c r="H66" s="11"/>
+      <c r="I66" s="11"/>
+      <c r="J66" s="11"/>
+      <c r="K66" s="11"/>
+      <c r="L66" s="11"/>
+      <c r="M66" s="11"/>
+      <c r="N66" s="11"/>
+      <c r="O66" s="11"/>
+      <c r="P66" s="28"/>
+    </row>
+    <row r="67" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="11"/>
+      <c r="B67" s="11"/>
+      <c r="C67" s="11"/>
+      <c r="D67" s="11"/>
+      <c r="E67" s="11"/>
+      <c r="F67" s="11"/>
+      <c r="G67" s="11"/>
+      <c r="H67" s="11"/>
+      <c r="I67" s="11"/>
+      <c r="J67" s="11"/>
+      <c r="K67" s="11"/>
+      <c r="L67" s="11"/>
+      <c r="M67" s="11"/>
+      <c r="N67" s="11"/>
+      <c r="O67" s="11"/>
+      <c r="P67" s="28"/>
+    </row>
+    <row r="68" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="11"/>
+      <c r="B68" s="11"/>
+      <c r="C68" s="11"/>
+      <c r="D68" s="11"/>
+      <c r="E68" s="11"/>
+      <c r="F68" s="11"/>
+      <c r="G68" s="11"/>
+      <c r="H68" s="11"/>
+      <c r="I68" s="11"/>
+      <c r="J68" s="11"/>
+      <c r="K68" s="11"/>
+      <c r="L68" s="11"/>
+      <c r="M68" s="11"/>
+      <c r="N68" s="11"/>
+      <c r="O68" s="11"/>
+      <c r="P68" s="28"/>
+    </row>
+    <row r="69" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="11"/>
+      <c r="B69" s="11"/>
+      <c r="C69" s="11"/>
+      <c r="D69" s="11"/>
+      <c r="E69" s="11"/>
+      <c r="F69" s="11"/>
+      <c r="G69" s="11"/>
+      <c r="H69" s="11"/>
+      <c r="I69" s="11"/>
+      <c r="J69" s="11"/>
+      <c r="K69" s="11"/>
+      <c r="L69" s="11"/>
+      <c r="M69" s="11"/>
+      <c r="N69" s="11"/>
+      <c r="O69" s="11"/>
+      <c r="P69" s="28"/>
+    </row>
+    <row r="70" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="11"/>
+      <c r="B70" s="11"/>
+      <c r="C70" s="11"/>
+      <c r="D70" s="11"/>
+      <c r="E70" s="11"/>
+      <c r="F70" s="11"/>
+      <c r="G70" s="11"/>
+      <c r="H70" s="11"/>
+      <c r="I70" s="11"/>
+      <c r="J70" s="11"/>
+      <c r="K70" s="11"/>
+      <c r="L70" s="11"/>
+      <c r="M70" s="11"/>
+      <c r="N70" s="11"/>
+      <c r="O70" s="11"/>
+      <c r="P70" s="28"/>
+    </row>
+    <row r="71" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="11"/>
+      <c r="B71" s="11"/>
+      <c r="C71" s="11"/>
+      <c r="D71" s="11"/>
+      <c r="E71" s="11"/>
+      <c r="F71" s="11"/>
+      <c r="G71" s="11"/>
+      <c r="H71" s="11"/>
+      <c r="I71" s="11"/>
+      <c r="J71" s="11"/>
+      <c r="K71" s="11"/>
+      <c r="L71" s="11"/>
+      <c r="M71" s="11"/>
+      <c r="N71" s="11"/>
+      <c r="O71" s="11"/>
+      <c r="P71" s="28"/>
+    </row>
+    <row r="72" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="11"/>
+      <c r="B72" s="11"/>
+      <c r="C72" s="11"/>
+      <c r="D72" s="11"/>
+      <c r="E72" s="11"/>
+      <c r="F72" s="11"/>
+      <c r="G72" s="11"/>
+      <c r="H72" s="11"/>
+      <c r="I72" s="11"/>
+      <c r="J72" s="11"/>
+      <c r="K72" s="11"/>
+      <c r="L72" s="11"/>
+      <c r="M72" s="11"/>
+      <c r="N72" s="11"/>
+      <c r="O72" s="11"/>
+      <c r="P72" s="28"/>
+    </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="12">
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A15:B15"/>
     <mergeCell ref="A16:B16"/>
@@ -1747,19 +2174,30 @@
     <mergeCell ref="A19:B19"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A26:D26"/>
+    <mergeCell ref="A29:D29"/>
+    <mergeCell ref="A53:P53"/>
+    <mergeCell ref="C54:I54"/>
+    <mergeCell ref="J54:P54"/>
   </mergeCells>
-  <dataValidations count="3">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B28:B41" type="list">
+  <dataValidations count="5">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B31:B44 B55:B68" type="list">
       <formula1>Groupes!$A$5:$A$11</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C28:C41" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C31:C44" type="list">
       <formula1>Groupes!$A$17:$A$21</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D28:D45" type="list">
-      <formula1>Groupes!$A$28:$A$45</formula1>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D31:D48" type="list">
+      <formula1>Groupes!$A$31:$A$48</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C55:I72" type="list">
+      <formula1>Groupes!$A$31:$A$48</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J55:P72" type="list">
+      <formula1>Groupes!$A$55:$A$72</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -1797,33 +2235,33 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="8" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="8" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="8" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="8" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="23" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="B5" s="23"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="23" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="AMG6" s="0"/>
       <c r="AMH6" s="0"/>
@@ -1832,31 +2270,31 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="23" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="B7" s="23"/>
     </row>
-    <row r="9" s="29" customFormat="true" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" s="31" customFormat="true" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1877,7 +2315,7 @@
       <c r="E11" s="11"/>
       <c r="F11" s="11"/>
       <c r="G11" s="11" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="J11" s="0"/>
     </row>
@@ -2157,222 +2595,222 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="30" width="9.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="32" width="9.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="8" width="19.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="30" width="10.05"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="4" style="30" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="32" width="10.05"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="4" style="32" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="32" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="32" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="32" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="32" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="33" t="s">
+        <v>72</v>
+      </c>
+      <c r="B5" s="34" t="n">
         <v>60</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="30" t="s">
+      <c r="C5" s="33" t="s">
+        <v>73</v>
+      </c>
+      <c r="D5" s="33" t="s">
+        <v>74</v>
+      </c>
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="35"/>
+      <c r="B6" s="35"/>
+      <c r="C6" s="33" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="D6" s="33" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="E6" s="33" t="n">
+        <v>0.416666666666667</v>
+      </c>
+      <c r="F6" s="33" t="n">
+        <v>0.458333333333333</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="36" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="36" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="30" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="30" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="B5" s="32" t="n">
-        <v>60</v>
-      </c>
-      <c r="C5" s="31" t="s">
-        <v>65</v>
-      </c>
-      <c r="D5" s="31" t="s">
-        <v>66</v>
-      </c>
-      <c r="E5" s="31"/>
-      <c r="F5" s="31"/>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="33"/>
-      <c r="B6" s="33"/>
-      <c r="C6" s="31" t="n">
-        <v>0.333333333333333</v>
-      </c>
-      <c r="D6" s="31" t="n">
-        <v>0.375</v>
-      </c>
-      <c r="E6" s="31" t="n">
-        <v>0.416666666666667</v>
-      </c>
-      <c r="F6" s="31" t="n">
-        <v>0.458333333333333</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="34" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="34" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="10" s="37" customFormat="true" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="35" t="s">
-        <v>68</v>
+    <row r="10" s="39" customFormat="true" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="37" t="s">
+        <v>76</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C10" s="36" t="s">
-        <v>70</v>
-      </c>
-      <c r="D10" s="36"/>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36"/>
-      <c r="G10" s="36"/>
-      <c r="H10" s="36"/>
-      <c r="I10" s="36"/>
+        <v>77</v>
+      </c>
+      <c r="C10" s="38" t="s">
+        <v>78</v>
+      </c>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="38"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="38"/>
+      <c r="A11" s="40"/>
       <c r="B11" s="28"/>
-      <c r="C11" s="38"/>
-      <c r="D11" s="38"/>
-      <c r="E11" s="38"/>
-      <c r="F11" s="38"/>
-      <c r="G11" s="38"/>
-      <c r="H11" s="38"/>
-      <c r="I11" s="38"/>
+      <c r="C11" s="40"/>
+      <c r="D11" s="40"/>
+      <c r="E11" s="40"/>
+      <c r="F11" s="40"/>
+      <c r="G11" s="40"/>
+      <c r="H11" s="40"/>
+      <c r="I11" s="40"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="39"/>
-      <c r="B12" s="39"/>
-      <c r="C12" s="38"/>
-      <c r="D12" s="38"/>
-      <c r="E12" s="38"/>
-      <c r="F12" s="38"/>
-      <c r="G12" s="38"/>
-      <c r="H12" s="38"/>
-      <c r="I12" s="38"/>
+      <c r="A12" s="41"/>
+      <c r="B12" s="41"/>
+      <c r="C12" s="40"/>
+      <c r="D12" s="40"/>
+      <c r="E12" s="40"/>
+      <c r="F12" s="40"/>
+      <c r="G12" s="40"/>
+      <c r="H12" s="40"/>
+      <c r="I12" s="40"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="38"/>
+      <c r="A13" s="40"/>
       <c r="B13" s="28"/>
-      <c r="C13" s="38"/>
-      <c r="D13" s="38"/>
-      <c r="E13" s="38"/>
-      <c r="F13" s="38"/>
-      <c r="G13" s="38"/>
-      <c r="H13" s="38"/>
-      <c r="I13" s="38"/>
+      <c r="C13" s="40"/>
+      <c r="D13" s="40"/>
+      <c r="E13" s="40"/>
+      <c r="F13" s="40"/>
+      <c r="G13" s="40"/>
+      <c r="H13" s="40"/>
+      <c r="I13" s="40"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="39"/>
-      <c r="B14" s="39"/>
-      <c r="C14" s="38"/>
-      <c r="D14" s="38"/>
-      <c r="E14" s="38"/>
-      <c r="F14" s="38"/>
-      <c r="G14" s="38"/>
-      <c r="H14" s="38"/>
-      <c r="I14" s="38"/>
+      <c r="A14" s="41"/>
+      <c r="B14" s="41"/>
+      <c r="C14" s="40"/>
+      <c r="D14" s="40"/>
+      <c r="E14" s="40"/>
+      <c r="F14" s="40"/>
+      <c r="G14" s="40"/>
+      <c r="H14" s="40"/>
+      <c r="I14" s="40"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="38"/>
+      <c r="A15" s="40"/>
       <c r="B15" s="28"/>
-      <c r="C15" s="38"/>
-      <c r="D15" s="38"/>
-      <c r="E15" s="38"/>
-      <c r="F15" s="38"/>
-      <c r="G15" s="38"/>
-      <c r="H15" s="38"/>
-      <c r="I15" s="38"/>
+      <c r="C15" s="40"/>
+      <c r="D15" s="40"/>
+      <c r="E15" s="40"/>
+      <c r="F15" s="40"/>
+      <c r="G15" s="40"/>
+      <c r="H15" s="40"/>
+      <c r="I15" s="40"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="39"/>
-      <c r="B16" s="39"/>
-      <c r="C16" s="38"/>
-      <c r="D16" s="38"/>
-      <c r="E16" s="38"/>
-      <c r="F16" s="38"/>
-      <c r="G16" s="38"/>
-      <c r="H16" s="38"/>
-      <c r="I16" s="38"/>
+      <c r="A16" s="41"/>
+      <c r="B16" s="41"/>
+      <c r="C16" s="40"/>
+      <c r="D16" s="40"/>
+      <c r="E16" s="40"/>
+      <c r="F16" s="40"/>
+      <c r="G16" s="40"/>
+      <c r="H16" s="40"/>
+      <c r="I16" s="40"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="38"/>
+      <c r="A17" s="40"/>
       <c r="B17" s="28"/>
-      <c r="C17" s="38"/>
-      <c r="D17" s="38"/>
-      <c r="E17" s="38"/>
-      <c r="F17" s="38"/>
-      <c r="G17" s="38"/>
-      <c r="H17" s="38"/>
-      <c r="I17" s="38"/>
+      <c r="C17" s="40"/>
+      <c r="D17" s="40"/>
+      <c r="E17" s="40"/>
+      <c r="F17" s="40"/>
+      <c r="G17" s="40"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="39"/>
-      <c r="B18" s="39"/>
-      <c r="C18" s="38"/>
-      <c r="D18" s="38"/>
-      <c r="E18" s="38"/>
-      <c r="F18" s="38"/>
-      <c r="G18" s="38"/>
-      <c r="H18" s="38"/>
-      <c r="I18" s="38"/>
+      <c r="A18" s="41"/>
+      <c r="B18" s="41"/>
+      <c r="C18" s="40"/>
+      <c r="D18" s="40"/>
+      <c r="E18" s="40"/>
+      <c r="F18" s="40"/>
+      <c r="G18" s="40"/>
+      <c r="H18" s="40"/>
+      <c r="I18" s="40"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="38"/>
+      <c r="A19" s="40"/>
       <c r="B19" s="28"/>
-      <c r="C19" s="38"/>
-      <c r="D19" s="38"/>
-      <c r="E19" s="38"/>
-      <c r="F19" s="38"/>
-      <c r="G19" s="38"/>
-      <c r="H19" s="38"/>
-      <c r="I19" s="38"/>
+      <c r="C19" s="40"/>
+      <c r="D19" s="40"/>
+      <c r="E19" s="40"/>
+      <c r="F19" s="40"/>
+      <c r="G19" s="40"/>
+      <c r="H19" s="40"/>
+      <c r="I19" s="40"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="39"/>
-      <c r="B20" s="39"/>
-      <c r="C20" s="38"/>
-      <c r="D20" s="38"/>
-      <c r="E20" s="38"/>
-      <c r="F20" s="38"/>
-      <c r="G20" s="38"/>
-      <c r="H20" s="38"/>
-      <c r="I20" s="38"/>
+      <c r="A20" s="41"/>
+      <c r="B20" s="41"/>
+      <c r="C20" s="40"/>
+      <c r="D20" s="40"/>
+      <c r="E20" s="40"/>
+      <c r="F20" s="40"/>
+      <c r="G20" s="40"/>
+      <c r="H20" s="40"/>
+      <c r="I20" s="40"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="38"/>
+      <c r="A21" s="40"/>
       <c r="B21" s="28"/>
-      <c r="C21" s="38"/>
-      <c r="D21" s="38"/>
-      <c r="E21" s="38"/>
-      <c r="F21" s="38"/>
-      <c r="G21" s="38"/>
-      <c r="H21" s="38"/>
-      <c r="I21" s="38"/>
+      <c r="C21" s="40"/>
+      <c r="D21" s="40"/>
+      <c r="E21" s="40"/>
+      <c r="F21" s="40"/>
+      <c r="G21" s="40"/>
+      <c r="H21" s="40"/>
+      <c r="I21" s="40"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="39"/>
-      <c r="B22" s="39"/>
-      <c r="C22" s="38"/>
-      <c r="D22" s="38"/>
-      <c r="E22" s="38"/>
-      <c r="F22" s="38"/>
-      <c r="G22" s="38"/>
-      <c r="H22" s="38"/>
-      <c r="I22" s="38"/>
+      <c r="A22" s="41"/>
+      <c r="B22" s="41"/>
+      <c r="C22" s="40"/>
+      <c r="D22" s="40"/>
+      <c r="E22" s="40"/>
+      <c r="F22" s="40"/>
+      <c r="G22" s="40"/>
+      <c r="H22" s="40"/>
+      <c r="I22" s="40"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>

<commit_message>
"deploy_database ok : sauf erreur de IntegrityError: insert or update on table "base_transversalgroup_conflicting_groups" violates foreign key constraint "base_transversalgrou_transversalgroup_id_d8ea42cd_fk_base_tran"
</commit_message>
<xml_diff>
--- a/FlOpEDT/media/configuration/empty_database_file.xlsx
+++ b/FlOpEDT/media/configuration/empty_database_file.xlsx
@@ -1512,8 +1512,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ72"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C15" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K15" activeCellId="0" sqref="K15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F51" activeCellId="0" sqref="F51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1521,7 +1521,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="8" width="16.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="8" width="29.5"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="8" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="8" width="11.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="8" width="11.64"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="5" style="8" width="11.52"/>
     <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="10" min="10" style="8" width="11.52"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1021" min="11" style="8" width="11.52"/>
@@ -1791,7 +1791,7 @@
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="23" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
debug transversal in deploy database
</commit_message>
<xml_diff>
--- a/FlOpEDT/media/configuration/empty_database_file.xlsx
+++ b/FlOpEDT/media/configuration/empty_database_file.xlsx
@@ -189,10 +189,10 @@
     <t xml:space="preserve">Groupes Transversaux</t>
   </si>
   <si>
-    <t xml:space="preserve">Transversal à quels groupes structuraux ?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Parallèle à quels groupes transversaux ?</t>
+    <t xml:space="preserve">Groupes structuraux en conflit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Groupes transversaux parallèles</t>
   </si>
   <si>
     <t xml:space="preserve">Un module est une charge d’enseignement sur une période et une promotion.</t>
@@ -1512,8 +1512,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ72"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F51" activeCellId="0" sqref="F51"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A18" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H47" activeCellId="0" sqref="H47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>